<commit_message>
ommit for WBS chages
</commit_message>
<xml_diff>
--- a/Uploader_WBS.xlsx
+++ b/Uploader_WBS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Study\Upload Engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Study\Upload Engine\Uploader-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Sr.</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Spring setup,caching setup, hibernate setup</t>
+  </si>
+  <si>
+    <t>GITHUB repository setup .</t>
+  </si>
+  <si>
+    <t>25-07-2016</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -611,102 +617,113 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>